<commit_message>
complete the code and now testing results
</commit_message>
<xml_diff>
--- a/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
+++ b/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,64 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>kingson@virogreenusa.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>info@horizontechnology.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>sales@horizontechnology.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>info@ctdi.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Usinfo@sproutup.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>600-4832info@TechWasteRecycling.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>info@techwasterecycling.com</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed unessesary prints. Changing append to += for list contatenation
</commit_message>
<xml_diff>
--- a/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
+++ b/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
@@ -413,14 +413,43 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>kingson@virogreenusa.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>info@horizontechnology.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sales@horizontechnology.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>info@ctdi.com</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed issue with filename
</commit_message>
<xml_diff>
--- a/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
+++ b/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,160 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Usinfo@sproutup.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>600-4832info@TechWasteRecycling.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>info@techwasterecycling.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>info@arrowrecovery.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Info@arrowrecovery.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>contact@baytechrecovery.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>info@bmionline.us</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>moe@datait.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Moe@datait.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>info@dgglobal.net</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>contact@evergreenitmanagement.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>info@greenland-resource.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>sales@ironsystems.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>info@ironsystems.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>info@magnakom.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>support@modernwastesolutions.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>onsiterecycling@myoer.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>info@poweron.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Andy@sem-recycling.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>info@smartwasteusa.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>goldy@starmicro.net</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>info@t3rs.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
removed useless stuff and fixed the file
</commit_message>
<xml_diff>
--- a/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
+++ b/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
@@ -413,197 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>kingson@virogreenusa.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>info@horizontechnology.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>sales@horizontechnology.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>info@ctdi.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Usinfo@sproutup.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>600-4832info@TechWasteRecycling.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>info@techwasterecycling.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>info@arrowrecovery.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Info@arrowrecovery.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>contact@baytechrecovery.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>info@bmionline.us</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>moe@datait.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Moe@datait.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>info@dgglobal.net</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>contact@evergreenitmanagement.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>info@greenland-resource.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>sales@ironsystems.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>info@ironsystems.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>info@magnakom.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>support@modernwastesolutions.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>onsiterecycling@myoer.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>info@poweron.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Andy@sem-recycling.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>info@smartwasteusa.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>goldy@starmicro.net</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>info@t3rs.com</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
patched up the excel document. Now committing and testing multiple files
</commit_message>
<xml_diff>
--- a/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
+++ b/webscraping/email-and-phone-scraper-master/emails_scrapped.xlsx
@@ -413,14 +413,50 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>kingson@virogreenusa.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sales@horizontechnology.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>info@horizontechnology.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>info@ctdi.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Usinfo@sproutup.com</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>